<commit_message>
:eagle: Add Robin game as core
</commit_message>
<xml_diff>
--- a/docs/Przykładowa rozgrywka.xlsx
+++ b/docs/Przykładowa rozgrywka.xlsx
@@ -1,22 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Cheshire\Documents\GitHub\robin-typescript\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FCEC1C-CB5B-4A94-85FF-2C033C881D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="23445" windowHeight="10320"/>
+    <workbookView xWindow="35580" yWindow="15" windowWidth="21105" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="119">
   <si>
     <t>PIERWSZA RUNDA</t>
   </si>
@@ -370,12 +388,15 @@
   </si>
   <si>
     <t>żeruj na utrzymanie kondycji</t>
+  </si>
+  <si>
+    <t>Modyfikator kształtu skrzydła</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -568,11 +589,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,6 +608,14 @@
       <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -633,7 +662,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -665,9 +694,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -699,6 +746,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -874,11 +939,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G776"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A738" workbookViewId="0">
-      <selection activeCell="L755" sqref="L755"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="H234" sqref="H234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -998,10 +1063,10 @@
       <c r="B15" s="9">
         <v>10</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="28">
         <v>4</v>
       </c>
-      <c r="E15" s="26"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="8" t="s">
@@ -1010,10 +1075,10 @@
       <c r="B16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="26"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="8" t="s">
@@ -1022,10 +1087,10 @@
       <c r="B17" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="26"/>
+      <c r="E17" s="28"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
@@ -1116,7 +1181,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D30" s="14">
         <v>0.05</v>
@@ -1252,10 +1317,10 @@
       <c r="B48" s="9">
         <v>5</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D48" s="28">
         <v>2</v>
       </c>
-      <c r="E48" s="26"/>
+      <c r="E48" s="28"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="8" t="s">
@@ -1264,10 +1329,10 @@
       <c r="B49" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="26" t="s">
+      <c r="D49" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E49" s="26"/>
+      <c r="E49" s="28"/>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="8" t="s">
@@ -1276,10 +1341,10 @@
       <c r="B50" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D50" s="26" t="s">
+      <c r="D50" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E50" s="26"/>
+      <c r="E50" s="28"/>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="6" t="s">
@@ -1417,10 +1482,10 @@
       <c r="B69" s="9">
         <v>9</v>
       </c>
-      <c r="D69" s="26">
+      <c r="D69" s="28">
         <v>10</v>
       </c>
-      <c r="E69" s="26"/>
+      <c r="E69" s="28"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="8" t="s">
@@ -1429,10 +1494,10 @@
       <c r="B70" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D70" s="26" t="s">
+      <c r="D70" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E70" s="26"/>
+      <c r="E70" s="28"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="8" t="s">
@@ -1441,10 +1506,10 @@
       <c r="B71" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D71" s="26" t="s">
+      <c r="D71" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E71" s="26"/>
+      <c r="E71" s="28"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="6" t="s">
@@ -1491,7 +1556,7 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D80" s="14">
         <v>0.05</v>
@@ -1624,7 +1689,7 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D100" s="14">
         <v>0.05</v>
@@ -1715,7 +1780,7 @@
       <c r="G110" s="13"/>
     </row>
     <row r="111" spans="1:7">
-      <c r="A111" s="27" t="s">
+      <c r="A111" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B111" s="19" t="s">
@@ -1803,10 +1868,10 @@
       <c r="B122" s="25">
         <v>12</v>
       </c>
-      <c r="D122" s="26">
+      <c r="D122" s="28">
         <v>13</v>
       </c>
-      <c r="E122" s="26"/>
+      <c r="E122" s="28"/>
     </row>
     <row r="123" spans="1:7">
       <c r="A123" s="8" t="s">
@@ -1815,10 +1880,10 @@
       <c r="B123" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D123" s="26" t="s">
+      <c r="D123" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E123" s="26"/>
+      <c r="E123" s="28"/>
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="8" t="s">
@@ -1827,10 +1892,10 @@
       <c r="B124" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D124" s="26" t="s">
+      <c r="D124" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E124" s="26"/>
+      <c r="E124" s="28"/>
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="6" t="s">
@@ -1929,7 +1994,7 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D138" s="14">
         <v>0.05</v>
@@ -2065,10 +2130,10 @@
       <c r="B156" s="25">
         <v>14</v>
       </c>
-      <c r="D156" s="26">
+      <c r="D156" s="28">
         <v>13</v>
       </c>
-      <c r="E156" s="26"/>
+      <c r="E156" s="28"/>
     </row>
     <row r="157" spans="1:7">
       <c r="A157" s="8" t="s">
@@ -2077,10 +2142,10 @@
       <c r="B157" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D157" s="26" t="s">
+      <c r="D157" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E157" s="26"/>
+      <c r="E157" s="28"/>
     </row>
     <row r="158" spans="1:7">
       <c r="A158" s="8" t="s">
@@ -2089,10 +2154,10 @@
       <c r="B158" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D158" s="26" t="s">
+      <c r="D158" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E158" s="26"/>
+      <c r="E158" s="28"/>
     </row>
     <row r="160" spans="1:7">
       <c r="A160" s="6" t="s">
@@ -2189,7 +2254,7 @@
     </row>
     <row r="172" spans="1:7">
       <c r="A172" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D172" s="14">
         <v>0.05</v>
@@ -2325,10 +2390,10 @@
       <c r="B190" s="25">
         <v>15</v>
       </c>
-      <c r="D190" s="26">
+      <c r="D190" s="28">
         <v>15</v>
       </c>
-      <c r="E190" s="26"/>
+      <c r="E190" s="28"/>
     </row>
     <row r="191" spans="1:7">
       <c r="A191" s="8" t="s">
@@ -2337,10 +2402,10 @@
       <c r="B191" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D191" s="26" t="s">
+      <c r="D191" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E191" s="26"/>
+      <c r="E191" s="28"/>
     </row>
     <row r="192" spans="1:7">
       <c r="A192" s="8" t="s">
@@ -2349,10 +2414,10 @@
       <c r="B192" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D192" s="26" t="s">
+      <c r="D192" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E192" s="26"/>
+      <c r="E192" s="28"/>
     </row>
     <row r="194" spans="1:7">
       <c r="A194" s="6" t="s">
@@ -2449,7 +2514,7 @@
     </row>
     <row r="206" spans="1:7">
       <c r="A206" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D206" s="14">
         <v>0.05</v>
@@ -2585,10 +2650,10 @@
       <c r="B224" s="25">
         <v>5</v>
       </c>
-      <c r="D224" s="26">
+      <c r="D224" s="28">
         <v>4</v>
       </c>
-      <c r="E224" s="26"/>
+      <c r="E224" s="28"/>
     </row>
     <row r="225" spans="1:7">
       <c r="A225" s="8" t="s">
@@ -2597,10 +2662,10 @@
       <c r="B225" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D225" s="26" t="s">
+      <c r="D225" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E225" s="26"/>
+      <c r="E225" s="28"/>
     </row>
     <row r="226" spans="1:7">
       <c r="A226" s="8" t="s">
@@ -2609,10 +2674,10 @@
       <c r="B226" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D226" s="26" t="s">
+      <c r="D226" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E226" s="26"/>
+      <c r="E226" s="28"/>
     </row>
     <row r="228" spans="1:7">
       <c r="A228" s="6" t="s">
@@ -2700,7 +2765,7 @@
     </row>
     <row r="239" spans="1:7">
       <c r="A239" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D239" s="14">
         <v>0.05</v>
@@ -2842,10 +2907,10 @@
       <c r="B258" s="25">
         <v>4</v>
       </c>
-      <c r="D258" s="26">
+      <c r="D258" s="28">
         <v>3</v>
       </c>
-      <c r="E258" s="26"/>
+      <c r="E258" s="28"/>
     </row>
     <row r="259" spans="1:7">
       <c r="A259" s="8" t="s">
@@ -2854,10 +2919,10 @@
       <c r="B259" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D259" s="26" t="s">
+      <c r="D259" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E259" s="26"/>
+      <c r="E259" s="28"/>
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="8" t="s">
@@ -2866,10 +2931,10 @@
       <c r="B260" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D260" s="26" t="s">
+      <c r="D260" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E260" s="26"/>
+      <c r="E260" s="28"/>
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="6" t="s">
@@ -2975,10 +3040,10 @@
       <c r="B277" s="25">
         <v>2</v>
       </c>
-      <c r="D277" s="26">
+      <c r="D277" s="28">
         <v>8</v>
       </c>
-      <c r="E277" s="26"/>
+      <c r="E277" s="28"/>
     </row>
     <row r="278" spans="1:7">
       <c r="A278" s="8" t="s">
@@ -2987,10 +3052,10 @@
       <c r="B278" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D278" s="26" t="s">
+      <c r="D278" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E278" s="26"/>
+      <c r="E278" s="28"/>
     </row>
     <row r="279" spans="1:7">
       <c r="A279" s="8" t="s">
@@ -2999,10 +3064,10 @@
       <c r="B279" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D279" s="26" t="s">
+      <c r="D279" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E279" s="26"/>
+      <c r="E279" s="28"/>
     </row>
     <row r="281" spans="1:7">
       <c r="A281" s="6" t="s">
@@ -3138,10 +3203,10 @@
       <c r="B299" s="25">
         <v>7</v>
       </c>
-      <c r="D299" s="26">
+      <c r="D299" s="28">
         <v>9</v>
       </c>
-      <c r="E299" s="26"/>
+      <c r="E299" s="28"/>
     </row>
     <row r="300" spans="1:7">
       <c r="A300" s="8" t="s">
@@ -3150,10 +3215,10 @@
       <c r="B300" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D300" s="26" t="s">
+      <c r="D300" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E300" s="26"/>
+      <c r="E300" s="28"/>
     </row>
     <row r="301" spans="1:7">
       <c r="A301" s="8" t="s">
@@ -3162,10 +3227,10 @@
       <c r="B301" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D301" s="26" t="s">
+      <c r="D301" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E301" s="26"/>
+      <c r="E301" s="28"/>
     </row>
     <row r="303" spans="1:7">
       <c r="A303" s="6" t="s">
@@ -3303,10 +3368,10 @@
       <c r="B320" s="25">
         <v>9</v>
       </c>
-      <c r="D320" s="26">
+      <c r="D320" s="28">
         <v>8</v>
       </c>
-      <c r="E320" s="26"/>
+      <c r="E320" s="28"/>
     </row>
     <row r="321" spans="1:5">
       <c r="A321" s="8" t="s">
@@ -3315,10 +3380,10 @@
       <c r="B321" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D321" s="26" t="s">
+      <c r="D321" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E321" s="26"/>
+      <c r="E321" s="28"/>
     </row>
     <row r="322" spans="1:5">
       <c r="A322" s="8" t="s">
@@ -3327,10 +3392,10 @@
       <c r="B322" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D322" s="26" t="s">
+      <c r="D322" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E322" s="26"/>
+      <c r="E322" s="28"/>
     </row>
     <row r="324" spans="1:5">
       <c r="A324" s="6" t="s">
@@ -3377,7 +3442,7 @@
     </row>
     <row r="331" spans="1:5">
       <c r="A331" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D331" s="14">
         <v>0.05</v>
@@ -3542,10 +3607,10 @@
       <c r="B352" s="25">
         <v>9</v>
       </c>
-      <c r="D352" s="26">
+      <c r="D352" s="28">
         <v>8</v>
       </c>
-      <c r="E352" s="26"/>
+      <c r="E352" s="28"/>
     </row>
     <row r="353" spans="1:7">
       <c r="A353" s="8" t="s">
@@ -3554,10 +3619,10 @@
       <c r="B353" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D353" s="26" t="s">
+      <c r="D353" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E353" s="26"/>
+      <c r="E353" s="28"/>
     </row>
     <row r="354" spans="1:7">
       <c r="A354" s="8" t="s">
@@ -3566,10 +3631,10 @@
       <c r="B354" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D354" s="26" t="s">
+      <c r="D354" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E354" s="26"/>
+      <c r="E354" s="28"/>
     </row>
     <row r="356" spans="1:7">
       <c r="A356" s="6" t="s">
@@ -3668,7 +3733,7 @@
     </row>
     <row r="368" spans="1:7">
       <c r="A368" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D368" s="14">
         <v>0.05</v>
@@ -3803,10 +3868,10 @@
       <c r="B386" s="25">
         <v>9</v>
       </c>
-      <c r="D386" s="26">
+      <c r="D386" s="28">
         <v>8</v>
       </c>
-      <c r="E386" s="26"/>
+      <c r="E386" s="28"/>
     </row>
     <row r="387" spans="1:7">
       <c r="A387" s="8" t="s">
@@ -3815,10 +3880,10 @@
       <c r="B387" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D387" s="26" t="s">
+      <c r="D387" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E387" s="26"/>
+      <c r="E387" s="28"/>
     </row>
     <row r="388" spans="1:7">
       <c r="A388" s="8" t="s">
@@ -3827,10 +3892,10 @@
       <c r="B388" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D388" s="26" t="s">
+      <c r="D388" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E388" s="26"/>
+      <c r="E388" s="28"/>
     </row>
     <row r="390" spans="1:7">
       <c r="A390" s="6" t="s">
@@ -3927,7 +3992,7 @@
     </row>
     <row r="402" spans="1:7">
       <c r="A402" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D402" s="14">
         <v>0.05</v>
@@ -4062,10 +4127,10 @@
       <c r="B420" s="25">
         <v>8</v>
       </c>
-      <c r="D420" s="26">
+      <c r="D420" s="28">
         <v>8</v>
       </c>
-      <c r="E420" s="26"/>
+      <c r="E420" s="28"/>
     </row>
     <row r="421" spans="1:7">
       <c r="A421" s="8" t="s">
@@ -4074,10 +4139,10 @@
       <c r="B421" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D421" s="26" t="s">
+      <c r="D421" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E421" s="26"/>
+      <c r="E421" s="28"/>
     </row>
     <row r="422" spans="1:7">
       <c r="A422" s="8" t="s">
@@ -4086,10 +4151,10 @@
       <c r="B422" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D422" s="26" t="s">
+      <c r="D422" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E422" s="26"/>
+      <c r="E422" s="28"/>
     </row>
     <row r="424" spans="1:7">
       <c r="A424" s="6" t="s">
@@ -4175,7 +4240,7 @@
     </row>
     <row r="435" spans="1:7">
       <c r="A435" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D435" s="14">
         <v>0.05</v>
@@ -4314,7 +4379,7 @@
     </row>
     <row r="455" spans="1:7">
       <c r="A455" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D455" s="14">
         <v>0.05</v>
@@ -4453,7 +4518,7 @@
     </row>
     <row r="475" spans="1:7">
       <c r="A475" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D475" s="14">
         <v>0.05</v>
@@ -4588,10 +4653,10 @@
       <c r="B493" s="25">
         <v>8</v>
       </c>
-      <c r="D493" s="26">
+      <c r="D493" s="28">
         <v>8</v>
       </c>
-      <c r="E493" s="26"/>
+      <c r="E493" s="28"/>
     </row>
     <row r="494" spans="1:7">
       <c r="A494" s="8" t="s">
@@ -4600,10 +4665,10 @@
       <c r="B494" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D494" s="26" t="s">
+      <c r="D494" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E494" s="26"/>
+      <c r="E494" s="28"/>
     </row>
     <row r="495" spans="1:7">
       <c r="A495" s="8" t="s">
@@ -4612,10 +4677,10 @@
       <c r="B495" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D495" s="26" t="s">
+      <c r="D495" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E495" s="26"/>
+      <c r="E495" s="28"/>
     </row>
     <row r="497" spans="1:7">
       <c r="A497" s="6" t="s">
@@ -4709,7 +4774,7 @@
     </row>
     <row r="508" spans="1:7">
       <c r="A508" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D508" s="14">
         <v>0.05</v>
@@ -4844,10 +4909,10 @@
       <c r="B526" s="25">
         <v>9</v>
       </c>
-      <c r="D526" s="26">
+      <c r="D526" s="28">
         <v>8</v>
       </c>
-      <c r="E526" s="26"/>
+      <c r="E526" s="28"/>
     </row>
     <row r="527" spans="1:7">
       <c r="A527" s="8" t="s">
@@ -4856,10 +4921,10 @@
       <c r="B527" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D527" s="26" t="s">
+      <c r="D527" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E527" s="26"/>
+      <c r="E527" s="28"/>
     </row>
     <row r="528" spans="1:7">
       <c r="A528" s="8" t="s">
@@ -4868,10 +4933,10 @@
       <c r="B528" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D528" s="26" t="s">
+      <c r="D528" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E528" s="26"/>
+      <c r="E528" s="28"/>
     </row>
     <row r="530" spans="1:7">
       <c r="A530" s="6" t="s">
@@ -4970,7 +5035,7 @@
     </row>
     <row r="542" spans="1:7">
       <c r="A542" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D542" s="14">
         <v>0.05</v>
@@ -5105,10 +5170,10 @@
       <c r="B560" s="25">
         <v>9</v>
       </c>
-      <c r="D560" s="26">
+      <c r="D560" s="28">
         <v>13</v>
       </c>
-      <c r="E560" s="26"/>
+      <c r="E560" s="28"/>
     </row>
     <row r="561" spans="1:7">
       <c r="A561" s="8" t="s">
@@ -5117,10 +5182,10 @@
       <c r="B561" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D561" s="26" t="s">
+      <c r="D561" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E561" s="26"/>
+      <c r="E561" s="28"/>
     </row>
     <row r="562" spans="1:7">
       <c r="A562" s="8" t="s">
@@ -5129,10 +5194,10 @@
       <c r="B562" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D562" s="26" t="s">
+      <c r="D562" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E562" s="26"/>
+      <c r="E562" s="28"/>
     </row>
     <row r="564" spans="1:7">
       <c r="A564" s="6" t="s">
@@ -5229,7 +5294,7 @@
     </row>
     <row r="576" spans="1:7">
       <c r="A576" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D576" s="14">
         <v>0.05</v>
@@ -5364,10 +5429,10 @@
       <c r="B594" s="25">
         <v>11</v>
       </c>
-      <c r="D594" s="26">
+      <c r="D594" s="28">
         <v>13</v>
       </c>
-      <c r="E594" s="26"/>
+      <c r="E594" s="28"/>
     </row>
     <row r="595" spans="1:7">
       <c r="A595" s="8" t="s">
@@ -5376,10 +5441,10 @@
       <c r="B595" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D595" s="26" t="s">
+      <c r="D595" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E595" s="26"/>
+      <c r="E595" s="28"/>
     </row>
     <row r="596" spans="1:7">
       <c r="A596" s="8" t="s">
@@ -5388,10 +5453,10 @@
       <c r="B596" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D596" s="26" t="s">
+      <c r="D596" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E596" s="26"/>
+      <c r="E596" s="28"/>
     </row>
     <row r="598" spans="1:7">
       <c r="A598" s="6" t="s">
@@ -5534,10 +5599,10 @@
       <c r="B616" s="25">
         <v>14</v>
       </c>
-      <c r="D616" s="26">
+      <c r="D616" s="28">
         <v>16</v>
       </c>
-      <c r="E616" s="26"/>
+      <c r="E616" s="28"/>
     </row>
     <row r="617" spans="1:7">
       <c r="A617" s="8" t="s">
@@ -5546,10 +5611,10 @@
       <c r="B617" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D617" s="26" t="s">
+      <c r="D617" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E617" s="26"/>
+      <c r="E617" s="28"/>
     </row>
     <row r="618" spans="1:7">
       <c r="A618" s="8" t="s">
@@ -5558,16 +5623,16 @@
       <c r="B618" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D618" s="26" t="s">
+      <c r="D618" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E618" s="26"/>
+      <c r="E618" s="28"/>
     </row>
     <row r="620" spans="1:7">
       <c r="A620" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B620" s="28">
+      <c r="B620" s="27">
         <v>5</v>
       </c>
     </row>
@@ -5653,10 +5718,10 @@
       <c r="B632" s="25">
         <v>15</v>
       </c>
-      <c r="D632" s="26">
+      <c r="D632" s="28">
         <v>16</v>
       </c>
-      <c r="E632" s="26"/>
+      <c r="E632" s="28"/>
     </row>
     <row r="633" spans="1:5">
       <c r="A633" s="8" t="s">
@@ -5665,10 +5730,10 @@
       <c r="B633" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D633" s="26" t="s">
+      <c r="D633" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E633" s="26"/>
+      <c r="E633" s="28"/>
     </row>
     <row r="634" spans="1:5">
       <c r="A634" s="8" t="s">
@@ -5677,10 +5742,10 @@
       <c r="B634" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D634" s="26" t="s">
+      <c r="D634" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E634" s="26"/>
+      <c r="E634" s="28"/>
     </row>
     <row r="636" spans="1:5">
       <c r="A636" s="6" t="s">
@@ -5786,10 +5851,10 @@
       <c r="B651" s="25">
         <v>15</v>
       </c>
-      <c r="D651" s="26">
+      <c r="D651" s="28">
         <v>17</v>
       </c>
-      <c r="E651" s="26"/>
+      <c r="E651" s="28"/>
     </row>
     <row r="652" spans="1:7">
       <c r="A652" s="8" t="s">
@@ -5798,10 +5863,10 @@
       <c r="B652" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D652" s="26" t="s">
+      <c r="D652" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E652" s="26"/>
+      <c r="E652" s="28"/>
     </row>
     <row r="653" spans="1:7">
       <c r="A653" s="8" t="s">
@@ -5810,10 +5875,10 @@
       <c r="B653" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D653" s="26" t="s">
+      <c r="D653" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E653" s="26"/>
+      <c r="E653" s="28"/>
     </row>
     <row r="655" spans="1:7">
       <c r="A655" s="6" t="s">
@@ -5912,7 +5977,7 @@
     </row>
     <row r="667" spans="1:7">
       <c r="A667" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D667" s="14">
         <v>0.05</v>
@@ -6047,10 +6112,10 @@
       <c r="B685" s="25">
         <v>17</v>
       </c>
-      <c r="D685" s="26">
+      <c r="D685" s="28">
         <v>16</v>
       </c>
-      <c r="E685" s="26"/>
+      <c r="E685" s="28"/>
     </row>
     <row r="686" spans="1:7">
       <c r="A686" s="8" t="s">
@@ -6059,10 +6124,10 @@
       <c r="B686" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D686" s="26" t="s">
+      <c r="D686" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E686" s="26"/>
+      <c r="E686" s="28"/>
     </row>
     <row r="687" spans="1:7">
       <c r="A687" s="8" t="s">
@@ -6071,10 +6136,10 @@
       <c r="B687" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D687" s="26" t="s">
+      <c r="D687" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E687" s="26"/>
+      <c r="E687" s="28"/>
     </row>
     <row r="689" spans="1:7">
       <c r="A689" s="6" t="s">
@@ -6171,7 +6236,7 @@
     </row>
     <row r="701" spans="1:7">
       <c r="A701" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D701" s="14">
         <v>0.05</v>
@@ -6306,10 +6371,10 @@
       <c r="B719" s="25">
         <v>17</v>
       </c>
-      <c r="D719" s="26">
+      <c r="D719" s="28">
         <v>12</v>
       </c>
-      <c r="E719" s="26"/>
+      <c r="E719" s="28"/>
     </row>
     <row r="720" spans="1:7">
       <c r="A720" s="8" t="s">
@@ -6318,10 +6383,10 @@
       <c r="B720" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D720" s="26" t="s">
+      <c r="D720" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E720" s="26"/>
+      <c r="E720" s="28"/>
     </row>
     <row r="721" spans="1:7">
       <c r="A721" s="8" t="s">
@@ -6330,10 +6395,10 @@
       <c r="B721" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D721" s="26" t="s">
+      <c r="D721" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="E721" s="26"/>
+      <c r="E721" s="28"/>
     </row>
     <row r="723" spans="1:7">
       <c r="A723" s="6" t="s">
@@ -6430,7 +6495,7 @@
     </row>
     <row r="735" spans="1:7">
       <c r="A735" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D735" s="14">
         <v>0.05</v>
@@ -6565,10 +6630,10 @@
       <c r="B753" s="25">
         <v>17</v>
       </c>
-      <c r="D753" s="26">
+      <c r="D753" s="28">
         <v>16</v>
       </c>
-      <c r="E753" s="26"/>
+      <c r="E753" s="28"/>
     </row>
     <row r="754" spans="1:7">
       <c r="A754" s="8" t="s">
@@ -6577,10 +6642,10 @@
       <c r="B754" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D754" s="26" t="s">
+      <c r="D754" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E754" s="26"/>
+      <c r="E754" s="28"/>
     </row>
     <row r="755" spans="1:7">
       <c r="A755" s="8" t="s">
@@ -6589,10 +6654,10 @@
       <c r="B755" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D755" s="26" t="s">
+      <c r="D755" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="E755" s="26"/>
+      <c r="E755" s="28"/>
     </row>
     <row r="757" spans="1:7">
       <c r="A757" s="6" t="s">
@@ -6689,7 +6754,7 @@
     </row>
     <row r="769" spans="1:5">
       <c r="A769" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="D769" s="14">
         <v>0.05</v>
@@ -6752,8 +6817,6 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="D721:E721"/>
-    <mergeCell ref="D753:E753"/>
     <mergeCell ref="D754:E754"/>
     <mergeCell ref="D755:E755"/>
     <mergeCell ref="D685:E685"/>
@@ -6761,11 +6824,11 @@
     <mergeCell ref="D687:E687"/>
     <mergeCell ref="D719:E719"/>
     <mergeCell ref="D720:E720"/>
-    <mergeCell ref="D561:E561"/>
-    <mergeCell ref="D562:E562"/>
     <mergeCell ref="D616:E616"/>
     <mergeCell ref="D617:E617"/>
     <mergeCell ref="D618:E618"/>
+    <mergeCell ref="D721:E721"/>
+    <mergeCell ref="D753:E753"/>
     <mergeCell ref="D386:E386"/>
     <mergeCell ref="D420:E420"/>
     <mergeCell ref="D493:E493"/>
@@ -6774,11 +6837,14 @@
     <mergeCell ref="D123:E123"/>
     <mergeCell ref="D124:E124"/>
     <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D632:E632"/>
-    <mergeCell ref="D633:E633"/>
-    <mergeCell ref="D634:E634"/>
-    <mergeCell ref="D651:E651"/>
-    <mergeCell ref="D652:E652"/>
+    <mergeCell ref="D322:E322"/>
+    <mergeCell ref="D353:E353"/>
+    <mergeCell ref="D354:E354"/>
+    <mergeCell ref="D387:E387"/>
+    <mergeCell ref="D388:E388"/>
+    <mergeCell ref="D421:E421"/>
+    <mergeCell ref="D422:E422"/>
+    <mergeCell ref="D352:E352"/>
     <mergeCell ref="D653:E653"/>
     <mergeCell ref="D594:E594"/>
     <mergeCell ref="D595:E595"/>
@@ -6788,14 +6854,13 @@
     <mergeCell ref="D527:E527"/>
     <mergeCell ref="D528:E528"/>
     <mergeCell ref="D560:E560"/>
-    <mergeCell ref="D322:E322"/>
-    <mergeCell ref="D353:E353"/>
-    <mergeCell ref="D354:E354"/>
-    <mergeCell ref="D387:E387"/>
-    <mergeCell ref="D388:E388"/>
-    <mergeCell ref="D421:E421"/>
-    <mergeCell ref="D422:E422"/>
-    <mergeCell ref="D352:E352"/>
+    <mergeCell ref="D632:E632"/>
+    <mergeCell ref="D633:E633"/>
+    <mergeCell ref="D634:E634"/>
+    <mergeCell ref="D651:E651"/>
+    <mergeCell ref="D652:E652"/>
+    <mergeCell ref="D561:E561"/>
+    <mergeCell ref="D562:E562"/>
     <mergeCell ref="D321:E321"/>
     <mergeCell ref="D226:E226"/>
     <mergeCell ref="D258:E258"/>
@@ -6815,15 +6880,15 @@
     <mergeCell ref="D190:E190"/>
     <mergeCell ref="D191:E191"/>
     <mergeCell ref="D192:E192"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6831,7 +6896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A36:G68"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -6914,10 +6979,10 @@
       <c r="B45" s="25">
         <v>17</v>
       </c>
-      <c r="D45" s="26">
+      <c r="D45" s="28">
         <v>16</v>
       </c>
-      <c r="E45" s="26"/>
+      <c r="E45" s="28"/>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="8" t="s">
@@ -6926,10 +6991,10 @@
       <c r="B46" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D46" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="26"/>
+      <c r="E46" s="28"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="8" t="s">
@@ -6938,10 +7003,10 @@
       <c r="B47" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D47" s="26" t="s">
+      <c r="D47" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="26"/>
+      <c r="E47" s="28"/>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="6" t="s">
@@ -7110,7 +7175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>